<commit_message>
Update languages code and name
</commit_message>
<xml_diff>
--- a/Dictionaries.xlsx
+++ b/Dictionaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loctv/Downloads/spell/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A99AE150-FC98-BE49-BFD0-055C59EA2D13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F353A0-B831-6A43-8FE7-845C630BA0FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{9AA42C21-5465-B44C-B48E-99B3E86BC8C3}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>dictionary-en</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
     <t>(MIT AND BSD)</t>
   </si>
   <si>
@@ -684,9 +681,6 @@
     <t>el-polyton</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
     <t>en-au</t>
   </si>
   <si>
@@ -922,13 +916,19 @@
   </si>
   <si>
     <t>vi</t>
+  </si>
+  <si>
+    <t>en_us</t>
+  </si>
+  <si>
+    <t>English (United States)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -949,6 +949,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -972,10 +978,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1291,19 +1298,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5DA2AA-B887-2E43-88FB-05FC0D584D7B}">
-  <dimension ref="A1:F788"/>
+  <dimension ref="A1:I788"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="82.5" customWidth="1"/>
-    <col min="2" max="2" width="64.5" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.83203125" customWidth="1"/>
+    <col min="6" max="6" width="38.1640625" customWidth="1"/>
+    <col min="7" max="7" width="34.1640625" customWidth="1"/>
+    <col min="9" max="9" width="34.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,14 +1324,26 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F1" t="str">
         <f>CONCATENATE(B1,"(",E1,")")</f>
         <v>Bulgarian(bg)</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G1" t="str">
+        <f>CONCATENATE(E1,": ",CHAR(34),B1,CHAR(34),",")</f>
+        <v>bg: "Bulgarian",</v>
+      </c>
+      <c r="H1" t="str">
+        <f>SUBSTITUTE(E1,"-","_")</f>
+        <v>bg</v>
+      </c>
+      <c r="I1" t="str">
+        <f>CONCATENATE(H1,": ",CHAR(34),B1,CHAR(34),",")</f>
+        <v>bg: "Bulgarian",</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1332,14 +1354,26 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F65" si="0">CONCATENATE(B2,"(",E2,")")</f>
         <v>Breton(br)</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <f>CONCATENATE(E2,": ",CHAR(34),B2,CHAR(34),",")</f>
+        <v>br: "Breton",</v>
+      </c>
+      <c r="H2" t="str">
+        <f>SUBSTITUTE(E2,"-","_")</f>
+        <v>br</v>
+      </c>
+      <c r="I2" t="str">
+        <f>CONCATENATE(H2,": ",CHAR(34),B2,CHAR(34),",")</f>
+        <v>br: "Breton",</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1350,14 +1384,26 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
         <v>Catalan(ca)</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f>CONCATENATE(E3,": ",CHAR(34),B3,CHAR(34),",")</f>
+        <v>ca: "Catalan",</v>
+      </c>
+      <c r="H3" t="str">
+        <f>SUBSTITUTE(E3,"-","_")</f>
+        <v>ca</v>
+      </c>
+      <c r="I3" t="str">
+        <f>CONCATENATE(H3,": ",CHAR(34),B3,CHAR(34),",")</f>
+        <v>ca: "Catalan",</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1368,14 +1414,26 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>Catalan (Valencian)(ca-valencia)</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f>CONCATENATE(E4,": ",CHAR(34),B4,CHAR(34),",")</f>
+        <v>ca-valencia: "Catalan (Valencian)",</v>
+      </c>
+      <c r="H4" t="str">
+        <f>SUBSTITUTE(E4,"-","_")</f>
+        <v>ca_valencia</v>
+      </c>
+      <c r="I4" t="str">
+        <f>CONCATENATE(H4,": ",CHAR(34),B4,CHAR(34),",")</f>
+        <v>ca_valencia: "Catalan (Valencian)",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1386,14 +1444,26 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>Czech(cs)</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f>CONCATENATE(E5,": ",CHAR(34),B5,CHAR(34),",")</f>
+        <v>cs: "Czech",</v>
+      </c>
+      <c r="H5" t="str">
+        <f>SUBSTITUTE(E5,"-","_")</f>
+        <v>cs</v>
+      </c>
+      <c r="I5" t="str">
+        <f>CONCATENATE(H5,": ",CHAR(34),B5,CHAR(34),",")</f>
+        <v>cs: "Czech",</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1404,14 +1474,26 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>Welsh(cy)</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G6" t="str">
+        <f>CONCATENATE(E6,": ",CHAR(34),B6,CHAR(34),",")</f>
+        <v>cy: "Welsh",</v>
+      </c>
+      <c r="H6" t="str">
+        <f>SUBSTITUTE(E6,"-","_")</f>
+        <v>cy</v>
+      </c>
+      <c r="I6" t="str">
+        <f>CONCATENATE(H6,": ",CHAR(34),B6,CHAR(34),",")</f>
+        <v>cy: "Welsh",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1422,14 +1504,26 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>Danish(da)</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G7" t="str">
+        <f>CONCATENATE(E7,": ",CHAR(34),B7,CHAR(34),",")</f>
+        <v>da: "Danish",</v>
+      </c>
+      <c r="H7" t="str">
+        <f>SUBSTITUTE(E7,"-","_")</f>
+        <v>da</v>
+      </c>
+      <c r="I7" t="str">
+        <f>CONCATENATE(H7,": ",CHAR(34),B7,CHAR(34),",")</f>
+        <v>da: "Danish",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1440,14 +1534,26 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v>German(de)</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G8" t="str">
+        <f>CONCATENATE(E8,": ",CHAR(34),B8,CHAR(34),",")</f>
+        <v>de: "German",</v>
+      </c>
+      <c r="H8" t="str">
+        <f>SUBSTITUTE(E8,"-","_")</f>
+        <v>de</v>
+      </c>
+      <c r="I8" t="str">
+        <f>CONCATENATE(H8,": ",CHAR(34),B8,CHAR(34),",")</f>
+        <v>de: "German",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1458,14 +1564,26 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v>German (Austria)(de-at)</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G9" t="str">
+        <f>CONCATENATE(E9,": ",CHAR(34),B9,CHAR(34),",")</f>
+        <v>de-at: "German (Austria)",</v>
+      </c>
+      <c r="H9" t="str">
+        <f>SUBSTITUTE(E9,"-","_")</f>
+        <v>de_at</v>
+      </c>
+      <c r="I9" t="str">
+        <f>CONCATENATE(H9,": ",CHAR(34),B9,CHAR(34),",")</f>
+        <v>de_at: "German (Austria)",</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -1476,14 +1594,26 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v>German (Switzerland)(de-ch)</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G10" t="str">
+        <f>CONCATENATE(E10,": ",CHAR(34),B10,CHAR(34),",")</f>
+        <v>de-ch: "German (Switzerland)",</v>
+      </c>
+      <c r="H10" t="str">
+        <f>SUBSTITUTE(E10,"-","_")</f>
+        <v>de_ch</v>
+      </c>
+      <c r="I10" t="str">
+        <f>CONCATENATE(H10,": ",CHAR(34),B10,CHAR(34),",")</f>
+        <v>de_ch: "German (Switzerland)",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -1494,14 +1624,26 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v>Modern Greek(el)</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G11" t="str">
+        <f>CONCATENATE(E11,": ",CHAR(34),B11,CHAR(34),",")</f>
+        <v>el: "Modern Greek",</v>
+      </c>
+      <c r="H11" t="str">
+        <f>SUBSTITUTE(E11,"-","_")</f>
+        <v>el</v>
+      </c>
+      <c r="I11" t="str">
+        <f>CONCATENATE(H11,": ",CHAR(34),B11,CHAR(34),",")</f>
+        <v>el: "Modern Greek",</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1512,1568 +1654,2684 @@
         <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
         <v>Modern Greek (Polytonic Greek)(el-polyton)</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G12" t="str">
+        <f>CONCATENATE(E12,": ",CHAR(34),B12,CHAR(34),",")</f>
+        <v>el-polyton: "Modern Greek (Polytonic Greek)",</v>
+      </c>
+      <c r="H12" t="str">
+        <f>SUBSTITUTE(E12,"-","_")</f>
+        <v>el_polyton</v>
+      </c>
+      <c r="I12" t="str">
+        <f>CONCATENATE(H12,": ",CHAR(34),B12,CHAR(34),",")</f>
+        <v>el_polyton: "Modern Greek (Polytonic Greek)",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="E13" t="s">
-        <v>219</v>
+        <v>297</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>English(en)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+        <v>English (United States)(en_us)</v>
+      </c>
+      <c r="G13" t="str">
+        <f>CONCATENATE(E13,": ",CHAR(34),B13,CHAR(34),",")</f>
+        <v>en_us: "English (United States)",</v>
+      </c>
+      <c r="H13" t="str">
+        <f>SUBSTITUTE(E13,"-","_")</f>
+        <v>en_us</v>
+      </c>
+      <c r="I13" t="str">
+        <f>CONCATENATE(H13,": ",CHAR(34),B13,CHAR(34),",")</f>
+        <v>en_us: "English (United States)",</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
         <v>English (Australia)(en-au)</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f>CONCATENATE(E14,": ",CHAR(34),B14,CHAR(34),",")</f>
+        <v>en-au: "English (Australia)",</v>
+      </c>
+      <c r="H14" t="str">
+        <f>SUBSTITUTE(E14,"-","_")</f>
+        <v>en_au</v>
+      </c>
+      <c r="I14" t="str">
+        <f>CONCATENATE(H14,": ",CHAR(34),B14,CHAR(34),",")</f>
+        <v>en_au: "English (Australia)",</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
         <v>English (Canada)(en-ca)</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G15" t="str">
+        <f>CONCATENATE(E15,": ",CHAR(34),B15,CHAR(34),",")</f>
+        <v>en-ca: "English (Canada)",</v>
+      </c>
+      <c r="H15" t="str">
+        <f>SUBSTITUTE(E15,"-","_")</f>
+        <v>en_ca</v>
+      </c>
+      <c r="I15" t="str">
+        <f>CONCATENATE(H15,": ",CHAR(34),B15,CHAR(34),",")</f>
+        <v>en_ca: "English (Canada)",</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
         <v>English (United Kingdom)(en-gb)</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f>CONCATENATE(E16,": ",CHAR(34),B16,CHAR(34),",")</f>
+        <v>en-gb: "English (United Kingdom)",</v>
+      </c>
+      <c r="H16" t="str">
+        <f>SUBSTITUTE(E16,"-","_")</f>
+        <v>en_gb</v>
+      </c>
+      <c r="I16" t="str">
+        <f>CONCATENATE(H16,": ",CHAR(34),B16,CHAR(34),",")</f>
+        <v>en_gb: "English (United Kingdom)",</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
         <v>English (South Africa)(en-za)</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G17" t="str">
+        <f>CONCATENATE(E17,": ",CHAR(34),B17,CHAR(34),",")</f>
+        <v>en-za: "English (South Africa)",</v>
+      </c>
+      <c r="H17" t="str">
+        <f>SUBSTITUTE(E17,"-","_")</f>
+        <v>en_za</v>
+      </c>
+      <c r="I17" t="str">
+        <f>CONCATENATE(H17,": ",CHAR(34),B17,CHAR(34),",")</f>
+        <v>en_za: "English (South Africa)",</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
         <v>Esperanto(eo)</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f>CONCATENATE(E18,": ",CHAR(34),B18,CHAR(34),",")</f>
+        <v>eo: "Esperanto",</v>
+      </c>
+      <c r="H18" t="str">
+        <f>SUBSTITUTE(E18,"-","_")</f>
+        <v>eo</v>
+      </c>
+      <c r="I18" t="str">
+        <f>CONCATENATE(H18,": ",CHAR(34),B18,CHAR(34),",")</f>
+        <v>eo: "Esperanto",</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian)(es)</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <f>CONCATENATE(E19,": ",CHAR(34),B19,CHAR(34),",")</f>
+        <v>es: "Spanish (or Castilian)",</v>
+      </c>
+      <c r="H19" t="str">
+        <f>SUBSTITUTE(E19,"-","_")</f>
+        <v>es</v>
+      </c>
+      <c r="I19" t="str">
+        <f>CONCATENATE(H19,": ",CHAR(34),B19,CHAR(34),",")</f>
+        <v>es: "Spanish (or Castilian)",</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Argentina)(es-ar)</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
+        <f>CONCATENATE(E20,": ",CHAR(34),B20,CHAR(34),",")</f>
+        <v>es-ar: "Spanish (or Castilian; Argentina)",</v>
+      </c>
+      <c r="H20" t="str">
+        <f>SUBSTITUTE(E20,"-","_")</f>
+        <v>es_ar</v>
+      </c>
+      <c r="I20" t="str">
+        <f>CONCATENATE(H20,": ",CHAR(34),B20,CHAR(34),",")</f>
+        <v>es_ar: "Spanish (or Castilian; Argentina)",</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Bolivia)(es-bo)</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G21" t="str">
+        <f>CONCATENATE(E21,": ",CHAR(34),B21,CHAR(34),",")</f>
+        <v>es-bo: "Spanish (or Castilian; Bolivia)",</v>
+      </c>
+      <c r="H21" t="str">
+        <f>SUBSTITUTE(E21,"-","_")</f>
+        <v>es_bo</v>
+      </c>
+      <c r="I21" t="str">
+        <f>CONCATENATE(H21,": ",CHAR(34),B21,CHAR(34),",")</f>
+        <v>es_bo: "Spanish (or Castilian; Bolivia)",</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Chile)(es-cl)</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G22" t="str">
+        <f>CONCATENATE(E22,": ",CHAR(34),B22,CHAR(34),",")</f>
+        <v>es-cl: "Spanish (or Castilian; Chile)",</v>
+      </c>
+      <c r="H22" t="str">
+        <f>SUBSTITUTE(E22,"-","_")</f>
+        <v>es_cl</v>
+      </c>
+      <c r="I22" t="str">
+        <f>CONCATENATE(H22,": ",CHAR(34),B22,CHAR(34),",")</f>
+        <v>es_cl: "Spanish (or Castilian; Chile)",</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Colombia)(es-co)</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G23" t="str">
+        <f>CONCATENATE(E23,": ",CHAR(34),B23,CHAR(34),",")</f>
+        <v>es-co: "Spanish (or Castilian; Colombia)",</v>
+      </c>
+      <c r="H23" t="str">
+        <f>SUBSTITUTE(E23,"-","_")</f>
+        <v>es_co</v>
+      </c>
+      <c r="I23" t="str">
+        <f>CONCATENATE(H23,": ",CHAR(34),B23,CHAR(34),",")</f>
+        <v>es_co: "Spanish (or Castilian; Colombia)",</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Costa Rica)(es-cr)</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G24" t="str">
+        <f>CONCATENATE(E24,": ",CHAR(34),B24,CHAR(34),",")</f>
+        <v>es-cr: "Spanish (or Castilian; Costa Rica)",</v>
+      </c>
+      <c r="H24" t="str">
+        <f>SUBSTITUTE(E24,"-","_")</f>
+        <v>es_cr</v>
+      </c>
+      <c r="I24" t="str">
+        <f>CONCATENATE(H24,": ",CHAR(34),B24,CHAR(34),",")</f>
+        <v>es_cr: "Spanish (or Castilian; Costa Rica)",</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Cuba)(es-cu)</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G25" t="str">
+        <f>CONCATENATE(E25,": ",CHAR(34),B25,CHAR(34),",")</f>
+        <v>es-cu: "Spanish (or Castilian; Cuba)",</v>
+      </c>
+      <c r="H25" t="str">
+        <f>SUBSTITUTE(E25,"-","_")</f>
+        <v>es_cu</v>
+      </c>
+      <c r="I25" t="str">
+        <f>CONCATENATE(H25,": ",CHAR(34),B25,CHAR(34),",")</f>
+        <v>es_cu: "Spanish (or Castilian; Cuba)",</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Dominican Republic)(es-do)</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G26" t="str">
+        <f>CONCATENATE(E26,": ",CHAR(34),B26,CHAR(34),",")</f>
+        <v>es-do: "Spanish (or Castilian; Dominican Republic)",</v>
+      </c>
+      <c r="H26" t="str">
+        <f>SUBSTITUTE(E26,"-","_")</f>
+        <v>es_do</v>
+      </c>
+      <c r="I26" t="str">
+        <f>CONCATENATE(H26,": ",CHAR(34),B26,CHAR(34),",")</f>
+        <v>es_do: "Spanish (or Castilian; Dominican Republic)",</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Ecuador)(es-ec)</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G27" t="str">
+        <f>CONCATENATE(E27,": ",CHAR(34),B27,CHAR(34),",")</f>
+        <v>es-ec: "Spanish (or Castilian; Ecuador)",</v>
+      </c>
+      <c r="H27" t="str">
+        <f>SUBSTITUTE(E27,"-","_")</f>
+        <v>es_ec</v>
+      </c>
+      <c r="I27" t="str">
+        <f>CONCATENATE(H27,": ",CHAR(34),B27,CHAR(34),",")</f>
+        <v>es_ec: "Spanish (or Castilian; Ecuador)",</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Guatemala)(es-gt)</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G28" t="str">
+        <f>CONCATENATE(E28,": ",CHAR(34),B28,CHAR(34),",")</f>
+        <v>es-gt: "Spanish (or Castilian; Guatemala)",</v>
+      </c>
+      <c r="H28" t="str">
+        <f>SUBSTITUTE(E28,"-","_")</f>
+        <v>es_gt</v>
+      </c>
+      <c r="I28" t="str">
+        <f>CONCATENATE(H28,": ",CHAR(34),B28,CHAR(34),",")</f>
+        <v>es_gt: "Spanish (or Castilian; Guatemala)",</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Honduras)(es-hn)</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G29" t="str">
+        <f>CONCATENATE(E29,": ",CHAR(34),B29,CHAR(34),",")</f>
+        <v>es-hn: "Spanish (or Castilian; Honduras)",</v>
+      </c>
+      <c r="H29" t="str">
+        <f>SUBSTITUTE(E29,"-","_")</f>
+        <v>es_hn</v>
+      </c>
+      <c r="I29" t="str">
+        <f>CONCATENATE(H29,": ",CHAR(34),B29,CHAR(34),",")</f>
+        <v>es_hn: "Spanish (or Castilian; Honduras)",</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Mexico)(es-mx)</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G30" t="str">
+        <f>CONCATENATE(E30,": ",CHAR(34),B30,CHAR(34),",")</f>
+        <v>es-mx: "Spanish (or Castilian; Mexico)",</v>
+      </c>
+      <c r="H30" t="str">
+        <f>SUBSTITUTE(E30,"-","_")</f>
+        <v>es_mx</v>
+      </c>
+      <c r="I30" t="str">
+        <f>CONCATENATE(H30,": ",CHAR(34),B30,CHAR(34),",")</f>
+        <v>es_mx: "Spanish (or Castilian; Mexico)",</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Nicaragua)(es-ni)</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G31" t="str">
+        <f>CONCATENATE(E31,": ",CHAR(34),B31,CHAR(34),",")</f>
+        <v>es-ni: "Spanish (or Castilian; Nicaragua)",</v>
+      </c>
+      <c r="H31" t="str">
+        <f>SUBSTITUTE(E31,"-","_")</f>
+        <v>es_ni</v>
+      </c>
+      <c r="I31" t="str">
+        <f>CONCATENATE(H31,": ",CHAR(34),B31,CHAR(34),",")</f>
+        <v>es_ni: "Spanish (or Castilian; Nicaragua)",</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Panama)(es-pa)</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G32" t="str">
+        <f>CONCATENATE(E32,": ",CHAR(34),B32,CHAR(34),",")</f>
+        <v>es-pa: "Spanish (or Castilian; Panama)",</v>
+      </c>
+      <c r="H32" t="str">
+        <f>SUBSTITUTE(E32,"-","_")</f>
+        <v>es_pa</v>
+      </c>
+      <c r="I32" t="str">
+        <f>CONCATENATE(H32,": ",CHAR(34),B32,CHAR(34),",")</f>
+        <v>es_pa: "Spanish (or Castilian; Panama)",</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Peru)(es-pe)</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G33" t="str">
+        <f>CONCATENATE(E33,": ",CHAR(34),B33,CHAR(34),",")</f>
+        <v>es-pe: "Spanish (or Castilian; Peru)",</v>
+      </c>
+      <c r="H33" t="str">
+        <f>SUBSTITUTE(E33,"-","_")</f>
+        <v>es_pe</v>
+      </c>
+      <c r="I33" t="str">
+        <f>CONCATENATE(H33,": ",CHAR(34),B33,CHAR(34),",")</f>
+        <v>es_pe: "Spanish (or Castilian; Peru)",</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Philippines)(es-ph)</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G34" t="str">
+        <f>CONCATENATE(E34,": ",CHAR(34),B34,CHAR(34),",")</f>
+        <v>es-ph: "Spanish (or Castilian; Philippines)",</v>
+      </c>
+      <c r="H34" t="str">
+        <f>SUBSTITUTE(E34,"-","_")</f>
+        <v>es_ph</v>
+      </c>
+      <c r="I34" t="str">
+        <f>CONCATENATE(H34,": ",CHAR(34),B34,CHAR(34),",")</f>
+        <v>es_ph: "Spanish (or Castilian; Philippines)",</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Puerto Rico)(es-pr)</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G35" t="str">
+        <f>CONCATENATE(E35,": ",CHAR(34),B35,CHAR(34),",")</f>
+        <v>es-pr: "Spanish (or Castilian; Puerto Rico)",</v>
+      </c>
+      <c r="H35" t="str">
+        <f>SUBSTITUTE(E35,"-","_")</f>
+        <v>es_pr</v>
+      </c>
+      <c r="I35" t="str">
+        <f>CONCATENATE(H35,": ",CHAR(34),B35,CHAR(34),",")</f>
+        <v>es_pr: "Spanish (or Castilian; Puerto Rico)",</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Paraguay)(es-py)</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G36" t="str">
+        <f>CONCATENATE(E36,": ",CHAR(34),B36,CHAR(34),",")</f>
+        <v>es-py: "Spanish (or Castilian; Paraguay)",</v>
+      </c>
+      <c r="H36" t="str">
+        <f>SUBSTITUTE(E36,"-","_")</f>
+        <v>es_py</v>
+      </c>
+      <c r="I36" t="str">
+        <f>CONCATENATE(H36,": ",CHAR(34),B36,CHAR(34),",")</f>
+        <v>es_py: "Spanish (or Castilian; Paraguay)",</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; El Salvador)(es-sv)</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G37" t="str">
+        <f>CONCATENATE(E37,": ",CHAR(34),B37,CHAR(34),",")</f>
+        <v>es-sv: "Spanish (or Castilian; El Salvador)",</v>
+      </c>
+      <c r="H37" t="str">
+        <f>SUBSTITUTE(E37,"-","_")</f>
+        <v>es_sv</v>
+      </c>
+      <c r="I37" t="str">
+        <f>CONCATENATE(H37,": ",CHAR(34),B37,CHAR(34),",")</f>
+        <v>es_sv: "Spanish (or Castilian; El Salvador)",</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E38" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; United States)(es-us)</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
+        <f>CONCATENATE(E38,": ",CHAR(34),B38,CHAR(34),",")</f>
+        <v>es-us: "Spanish (or Castilian; United States)",</v>
+      </c>
+      <c r="H38" t="str">
+        <f>SUBSTITUTE(E38,"-","_")</f>
+        <v>es_us</v>
+      </c>
+      <c r="I38" t="str">
+        <f>CONCATENATE(H38,": ",CHAR(34),B38,CHAR(34),",")</f>
+        <v>es_us: "Spanish (or Castilian; United States)",</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Uruguay)(es-uy)</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
+        <f>CONCATENATE(E39,": ",CHAR(34),B39,CHAR(34),",")</f>
+        <v>es-uy: "Spanish (or Castilian; Uruguay)",</v>
+      </c>
+      <c r="H39" t="str">
+        <f>SUBSTITUTE(E39,"-","_")</f>
+        <v>es_uy</v>
+      </c>
+      <c r="I39" t="str">
+        <f>CONCATENATE(H39,": ",CHAR(34),B39,CHAR(34),",")</f>
+        <v>es_uy: "Spanish (or Castilian; Uruguay)",</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
         <v>Spanish (or Castilian; Venezuela)(es-ve)</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G40" t="str">
+        <f>CONCATENATE(E40,": ",CHAR(34),B40,CHAR(34),",")</f>
+        <v>es-ve: "Spanish (or Castilian; Venezuela)",</v>
+      </c>
+      <c r="H40" t="str">
+        <f>SUBSTITUTE(E40,"-","_")</f>
+        <v>es_ve</v>
+      </c>
+      <c r="I40" t="str">
+        <f>CONCATENATE(H40,": ",CHAR(34),B40,CHAR(34),",")</f>
+        <v>es_ve: "Spanish (or Castilian; Venezuela)",</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E41" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
         <v>Estonian(et)</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G41" t="str">
+        <f>CONCATENATE(E41,": ",CHAR(34),B41,CHAR(34),",")</f>
+        <v>et: "Estonian",</v>
+      </c>
+      <c r="H41" t="str">
+        <f>SUBSTITUTE(E41,"-","_")</f>
+        <v>et</v>
+      </c>
+      <c r="I41" t="str">
+        <f>CONCATENATE(H41,": ",CHAR(34),B41,CHAR(34),",")</f>
+        <v>et: "Estonian",</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
         <v>Basque(eu)</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G42" t="str">
+        <f>CONCATENATE(E42,": ",CHAR(34),B42,CHAR(34),",")</f>
+        <v>eu: "Basque",</v>
+      </c>
+      <c r="H42" t="str">
+        <f>SUBSTITUTE(E42,"-","_")</f>
+        <v>eu</v>
+      </c>
+      <c r="I42" t="str">
+        <f>CONCATENATE(H42,": ",CHAR(34),B42,CHAR(34),",")</f>
+        <v>eu: "Basque",</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="E43" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
         <v>Persian(fa)</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G43" t="str">
+        <f>CONCATENATE(E43,": ",CHAR(34),B43,CHAR(34),",")</f>
+        <v>fa: "Persian",</v>
+      </c>
+      <c r="H43" t="str">
+        <f>SUBSTITUTE(E43,"-","_")</f>
+        <v>fa</v>
+      </c>
+      <c r="I43" t="str">
+        <f>CONCATENATE(H43,": ",CHAR(34),B43,CHAR(34),",")</f>
+        <v>fa: "Persian",</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E44" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
         <v>Faroese(fo)</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G44" t="str">
+        <f>CONCATENATE(E44,": ",CHAR(34),B44,CHAR(34),",")</f>
+        <v>fo: "Faroese",</v>
+      </c>
+      <c r="H44" t="str">
+        <f>SUBSTITUTE(E44,"-","_")</f>
+        <v>fo</v>
+      </c>
+      <c r="I44" t="str">
+        <f>CONCATENATE(H44,": ",CHAR(34),B44,CHAR(34),",")</f>
+        <v>fo: "Faroese",</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="E45" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
         <v>French(fr)</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G45" t="str">
+        <f>CONCATENATE(E45,": ",CHAR(34),B45,CHAR(34),",")</f>
+        <v>fr: "French",</v>
+      </c>
+      <c r="H45" t="str">
+        <f>SUBSTITUTE(E45,"-","_")</f>
+        <v>fr</v>
+      </c>
+      <c r="I45" t="str">
+        <f>CONCATENATE(H45,": ",CHAR(34),B45,CHAR(34),",")</f>
+        <v>fr: "French",</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
         <v>Friulian(fur)</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G46" t="str">
+        <f>CONCATENATE(E46,": ",CHAR(34),B46,CHAR(34),",")</f>
+        <v>fur: "Friulian",</v>
+      </c>
+      <c r="H46" t="str">
+        <f>SUBSTITUTE(E46,"-","_")</f>
+        <v>fur</v>
+      </c>
+      <c r="I46" t="str">
+        <f>CONCATENATE(H46,": ",CHAR(34),B46,CHAR(34),",")</f>
+        <v>fur: "Friulian",</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E47" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
         <v>Western Frisian(fy)</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G47" t="str">
+        <f>CONCATENATE(E47,": ",CHAR(34),B47,CHAR(34),",")</f>
+        <v>fy: "Western Frisian",</v>
+      </c>
+      <c r="H47" t="str">
+        <f>SUBSTITUTE(E47,"-","_")</f>
+        <v>fy</v>
+      </c>
+      <c r="I47" t="str">
+        <f>CONCATENATE(H47,": ",CHAR(34),B47,CHAR(34),",")</f>
+        <v>fy: "Western Frisian",</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
         <v>Irish(ga)</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G48" t="str">
+        <f>CONCATENATE(E48,": ",CHAR(34),B48,CHAR(34),",")</f>
+        <v>ga: "Irish",</v>
+      </c>
+      <c r="H48" t="str">
+        <f>SUBSTITUTE(E48,"-","_")</f>
+        <v>ga</v>
+      </c>
+      <c r="I48" t="str">
+        <f>CONCATENATE(H48,": ",CHAR(34),B48,CHAR(34),",")</f>
+        <v>ga: "Irish",</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E49" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
         <v>Scottish Gaelic (or Gaelic)(gd)</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G49" t="str">
+        <f>CONCATENATE(E49,": ",CHAR(34),B49,CHAR(34),",")</f>
+        <v>gd: "Scottish Gaelic (or Gaelic)",</v>
+      </c>
+      <c r="H49" t="str">
+        <f>SUBSTITUTE(E49,"-","_")</f>
+        <v>gd</v>
+      </c>
+      <c r="I49" t="str">
+        <f>CONCATENATE(H49,": ",CHAR(34),B49,CHAR(34),",")</f>
+        <v>gd: "Scottish Gaelic (or Gaelic)",</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E50" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
         <v>Galician(gl)</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G50" t="str">
+        <f>CONCATENATE(E50,": ",CHAR(34),B50,CHAR(34),",")</f>
+        <v>gl: "Galician",</v>
+      </c>
+      <c r="H50" t="str">
+        <f>SUBSTITUTE(E50,"-","_")</f>
+        <v>gl</v>
+      </c>
+      <c r="I50" t="str">
+        <f>CONCATENATE(H50,": ",CHAR(34),B50,CHAR(34),",")</f>
+        <v>gl: "Galician",</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="E51" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
         <v>Hebrew(he)</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G51" t="str">
+        <f>CONCATENATE(E51,": ",CHAR(34),B51,CHAR(34),",")</f>
+        <v>he: "Hebrew",</v>
+      </c>
+      <c r="H51" t="str">
+        <f>SUBSTITUTE(E51,"-","_")</f>
+        <v>he</v>
+      </c>
+      <c r="I51" t="str">
+        <f>CONCATENATE(H51,": ",CHAR(34),B51,CHAR(34),",")</f>
+        <v>he: "Hebrew",</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="E52" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
         <v>Croatian(hr)</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G52" t="str">
+        <f>CONCATENATE(E52,": ",CHAR(34),B52,CHAR(34),",")</f>
+        <v>hr: "Croatian",</v>
+      </c>
+      <c r="H52" t="str">
+        <f>SUBSTITUTE(E52,"-","_")</f>
+        <v>hr</v>
+      </c>
+      <c r="I52" t="str">
+        <f>CONCATENATE(H52,": ",CHAR(34),B52,CHAR(34),",")</f>
+        <v>hr: "Croatian",</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
         <v>Hungarian(hu)</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G53" t="str">
+        <f>CONCATENATE(E53,": ",CHAR(34),B53,CHAR(34),",")</f>
+        <v>hu: "Hungarian",</v>
+      </c>
+      <c r="H53" t="str">
+        <f>SUBSTITUTE(E53,"-","_")</f>
+        <v>hu</v>
+      </c>
+      <c r="I53" t="str">
+        <f>CONCATENATE(H53,": ",CHAR(34),B53,CHAR(34),",")</f>
+        <v>hu: "Hungarian",</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
         <v>Armenian(hy)</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G54" t="str">
+        <f>CONCATENATE(E54,": ",CHAR(34),B54,CHAR(34),",")</f>
+        <v>hy: "Armenian",</v>
+      </c>
+      <c r="H54" t="str">
+        <f>SUBSTITUTE(E54,"-","_")</f>
+        <v>hy</v>
+      </c>
+      <c r="I54" t="str">
+        <f>CONCATENATE(H54,": ",CHAR(34),B54,CHAR(34),",")</f>
+        <v>hy: "Armenian",</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
         <v>Western Armenian(hyw)</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G55" t="str">
+        <f>CONCATENATE(E55,": ",CHAR(34),B55,CHAR(34),",")</f>
+        <v>hyw: "Western Armenian",</v>
+      </c>
+      <c r="H55" t="str">
+        <f>SUBSTITUTE(E55,"-","_")</f>
+        <v>hyw</v>
+      </c>
+      <c r="I55" t="str">
+        <f>CONCATENATE(H55,": ",CHAR(34),B55,CHAR(34),",")</f>
+        <v>hyw: "Western Armenian",</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E56" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
         <v>Interlingua(ia)</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G56" t="str">
+        <f>CONCATENATE(E56,": ",CHAR(34),B56,CHAR(34),",")</f>
+        <v>ia: "Interlingua",</v>
+      </c>
+      <c r="H56" t="str">
+        <f>SUBSTITUTE(E56,"-","_")</f>
+        <v>ia</v>
+      </c>
+      <c r="I56" t="str">
+        <f>CONCATENATE(H56,": ",CHAR(34),B56,CHAR(34),",")</f>
+        <v>ia: "Interlingua",</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="C57" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E57" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
         <v>Interlingue (or Occidental)(ie)</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G57" t="str">
+        <f>CONCATENATE(E57,": ",CHAR(34),B57,CHAR(34),",")</f>
+        <v>ie: "Interlingue (or Occidental)",</v>
+      </c>
+      <c r="H57" t="str">
+        <f>SUBSTITUTE(E57,"-","_")</f>
+        <v>ie</v>
+      </c>
+      <c r="I57" t="str">
+        <f>CONCATENATE(H57,": ",CHAR(34),B57,CHAR(34),",")</f>
+        <v>ie: "Interlingue (or Occidental)",</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="E58" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
         <v>Icelandic(is)</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G58" t="str">
+        <f>CONCATENATE(E58,": ",CHAR(34),B58,CHAR(34),",")</f>
+        <v>is: "Icelandic",</v>
+      </c>
+      <c r="H58" t="str">
+        <f>SUBSTITUTE(E58,"-","_")</f>
+        <v>is</v>
+      </c>
+      <c r="I58" t="str">
+        <f>CONCATENATE(H58,": ",CHAR(34),B58,CHAR(34),",")</f>
+        <v>is: "Icelandic",</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E59" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
         <v>Italian(it)</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G59" t="str">
+        <f>CONCATENATE(E59,": ",CHAR(34),B59,CHAR(34),",")</f>
+        <v>it: "Italian",</v>
+      </c>
+      <c r="H59" t="str">
+        <f>SUBSTITUTE(E59,"-","_")</f>
+        <v>it</v>
+      </c>
+      <c r="I59" t="str">
+        <f>CONCATENATE(H59,": ",CHAR(34),B59,CHAR(34),",")</f>
+        <v>it: "Italian",</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="E60" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
         <v>Georgian(ka)</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G60" t="str">
+        <f>CONCATENATE(E60,": ",CHAR(34),B60,CHAR(34),",")</f>
+        <v>ka: "Georgian",</v>
+      </c>
+      <c r="H60" t="str">
+        <f>SUBSTITUTE(E60,"-","_")</f>
+        <v>ka</v>
+      </c>
+      <c r="I60" t="str">
+        <f>CONCATENATE(H60,": ",CHAR(34),B60,CHAR(34),",")</f>
+        <v>ka: "Georgian",</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
         <v>Korean(ko)</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G61" t="str">
+        <f>CONCATENATE(E61,": ",CHAR(34),B61,CHAR(34),",")</f>
+        <v>ko: "Korean",</v>
+      </c>
+      <c r="H61" t="str">
+        <f>SUBSTITUTE(E61,"-","_")</f>
+        <v>ko</v>
+      </c>
+      <c r="I61" t="str">
+        <f>CONCATENATE(H61,": ",CHAR(34),B61,CHAR(34),",")</f>
+        <v>ko: "Korean",</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E62" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
         <v>Latin(la)</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G62" t="str">
+        <f>CONCATENATE(E62,": ",CHAR(34),B62,CHAR(34),",")</f>
+        <v>la: "Latin",</v>
+      </c>
+      <c r="H62" t="str">
+        <f>SUBSTITUTE(E62,"-","_")</f>
+        <v>la</v>
+      </c>
+      <c r="I62" t="str">
+        <f>CONCATENATE(H62,": ",CHAR(34),B62,CHAR(34),",")</f>
+        <v>la: "Latin",</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="E63" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
         <v>Luxembourgish (or Letzeburgesch)(lb)</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G63" t="str">
+        <f>CONCATENATE(E63,": ",CHAR(34),B63,CHAR(34),",")</f>
+        <v>lb: "Luxembourgish (or Letzeburgesch)",</v>
+      </c>
+      <c r="H63" t="str">
+        <f>SUBSTITUTE(E63,"-","_")</f>
+        <v>lb</v>
+      </c>
+      <c r="I63" t="str">
+        <f>CONCATENATE(H63,": ",CHAR(34),B63,CHAR(34),",")</f>
+        <v>lb: "Luxembourgish (or Letzeburgesch)",</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="E64" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
         <v>Lithuanian(lt)</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G64" t="str">
+        <f>CONCATENATE(E64,": ",CHAR(34),B64,CHAR(34),",")</f>
+        <v>lt: "Lithuanian",</v>
+      </c>
+      <c r="H64" t="str">
+        <f>SUBSTITUTE(E64,"-","_")</f>
+        <v>lt</v>
+      </c>
+      <c r="I64" t="str">
+        <f>CONCATENATE(H64,": ",CHAR(34),B64,CHAR(34),",")</f>
+        <v>lt: "Lithuanian",</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="C65" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E65" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
         <v>Latgalian(ltg)</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G65" t="str">
+        <f>CONCATENATE(E65,": ",CHAR(34),B65,CHAR(34),",")</f>
+        <v>ltg: "Latgalian",</v>
+      </c>
+      <c r="H65" t="str">
+        <f>SUBSTITUTE(E65,"-","_")</f>
+        <v>ltg</v>
+      </c>
+      <c r="I65" t="str">
+        <f>CONCATENATE(H65,": ",CHAR(34),B65,CHAR(34),",")</f>
+        <v>ltg: "Latgalian",</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="C66" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E66" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" ref="F66:F129" si="1">CONCATENATE(B66,"(",E66,")")</f>
         <v>Latvian(lv)</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G66" t="str">
+        <f>CONCATENATE(E66,": ",CHAR(34),B66,CHAR(34),",")</f>
+        <v>lv: "Latvian",</v>
+      </c>
+      <c r="H66" t="str">
+        <f>SUBSTITUTE(E66,"-","_")</f>
+        <v>lv</v>
+      </c>
+      <c r="I66" t="str">
+        <f>CONCATENATE(H66,": ",CHAR(34),B66,CHAR(34),",")</f>
+        <v>lv: "Latvian",</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E67" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" si="1"/>
         <v>Macedonian(mk)</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G67" t="str">
+        <f>CONCATENATE(E67,": ",CHAR(34),B67,CHAR(34),",")</f>
+        <v>mk: "Macedonian",</v>
+      </c>
+      <c r="H67" t="str">
+        <f>SUBSTITUTE(E67,"-","_")</f>
+        <v>mk</v>
+      </c>
+      <c r="I67" t="str">
+        <f>CONCATENATE(H67,": ",CHAR(34),B67,CHAR(34),",")</f>
+        <v>mk: "Macedonian",</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="E68" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="1"/>
         <v>Mongolian(mn)</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G68" t="str">
+        <f>CONCATENATE(E68,": ",CHAR(34),B68,CHAR(34),",")</f>
+        <v>mn: "Mongolian",</v>
+      </c>
+      <c r="H68" t="str">
+        <f>SUBSTITUTE(E68,"-","_")</f>
+        <v>mn</v>
+      </c>
+      <c r="I68" t="str">
+        <f>CONCATENATE(H68,": ",CHAR(34),B68,CHAR(34),",")</f>
+        <v>mn: "Mongolian",</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="1"/>
         <v>Norwegian Bokmål(nb)</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G69" t="str">
+        <f>CONCATENATE(E69,": ",CHAR(34),B69,CHAR(34),",")</f>
+        <v>nb: "Norwegian Bokmål",</v>
+      </c>
+      <c r="H69" t="str">
+        <f>SUBSTITUTE(E69,"-","_")</f>
+        <v>nb</v>
+      </c>
+      <c r="I69" t="str">
+        <f>CONCATENATE(H69,": ",CHAR(34),B69,CHAR(34),",")</f>
+        <v>nb: "Norwegian Bokmål",</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E70" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="1"/>
         <v>Low German (or Low Saxon)(nds)</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G70" t="str">
+        <f>CONCATENATE(E70,": ",CHAR(34),B70,CHAR(34),",")</f>
+        <v>nds: "Low German (or Low Saxon)",</v>
+      </c>
+      <c r="H70" t="str">
+        <f>SUBSTITUTE(E70,"-","_")</f>
+        <v>nds</v>
+      </c>
+      <c r="I70" t="str">
+        <f>CONCATENATE(H70,": ",CHAR(34),B70,CHAR(34),",")</f>
+        <v>nds: "Low German (or Low Saxon)",</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="C71" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E71" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="1"/>
         <v>Nepali(ne)</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G71" t="str">
+        <f>CONCATENATE(E71,": ",CHAR(34),B71,CHAR(34),",")</f>
+        <v>ne: "Nepali",</v>
+      </c>
+      <c r="H71" t="str">
+        <f>SUBSTITUTE(E71,"-","_")</f>
+        <v>ne</v>
+      </c>
+      <c r="I71" t="str">
+        <f>CONCATENATE(H71,": ",CHAR(34),B71,CHAR(34),",")</f>
+        <v>ne: "Nepali",</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="E72" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="1"/>
         <v>Dutch (or Flemish)(nl)</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G72" t="str">
+        <f>CONCATENATE(E72,": ",CHAR(34),B72,CHAR(34),",")</f>
+        <v>nl: "Dutch (or Flemish)",</v>
+      </c>
+      <c r="H72" t="str">
+        <f>SUBSTITUTE(E72,"-","_")</f>
+        <v>nl</v>
+      </c>
+      <c r="I72" t="str">
+        <f>CONCATENATE(H72,": ",CHAR(34),B72,CHAR(34),",")</f>
+        <v>nl: "Dutch (or Flemish)",</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="1"/>
         <v>Norwegian Nynorsk(nn)</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G73" t="str">
+        <f>CONCATENATE(E73,": ",CHAR(34),B73,CHAR(34),",")</f>
+        <v>nn: "Norwegian Nynorsk",</v>
+      </c>
+      <c r="H73" t="str">
+        <f>SUBSTITUTE(E73,"-","_")</f>
+        <v>nn</v>
+      </c>
+      <c r="I73" t="str">
+        <f>CONCATENATE(H73,": ",CHAR(34),B73,CHAR(34),",")</f>
+        <v>nn: "Norwegian Nynorsk",</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="1"/>
         <v>Occitan (post 1500)(oc)</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G74" t="str">
+        <f>CONCATENATE(E74,": ",CHAR(34),B74,CHAR(34),",")</f>
+        <v>oc: "Occitan (post 1500)",</v>
+      </c>
+      <c r="H74" t="str">
+        <f>SUBSTITUTE(E74,"-","_")</f>
+        <v>oc</v>
+      </c>
+      <c r="I74" t="str">
+        <f>CONCATENATE(H74,": ",CHAR(34),B74,CHAR(34),",")</f>
+        <v>oc: "Occitan (post 1500)",</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E75" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="1"/>
         <v>Polish(pl)</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G75" t="str">
+        <f>CONCATENATE(E75,": ",CHAR(34),B75,CHAR(34),",")</f>
+        <v>pl: "Polish",</v>
+      </c>
+      <c r="H75" t="str">
+        <f>SUBSTITUTE(E75,"-","_")</f>
+        <v>pl</v>
+      </c>
+      <c r="I75" t="str">
+        <f>CONCATENATE(H75,": ",CHAR(34),B75,CHAR(34),",")</f>
+        <v>pl: "Polish",</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="E76" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="1"/>
         <v>Portuguese(pt)</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G76" t="str">
+        <f>CONCATENATE(E76,": ",CHAR(34),B76,CHAR(34),",")</f>
+        <v>pt: "Portuguese",</v>
+      </c>
+      <c r="H76" t="str">
+        <f>SUBSTITUTE(E76,"-","_")</f>
+        <v>pt</v>
+      </c>
+      <c r="I76" t="str">
+        <f>CONCATENATE(H76,": ",CHAR(34),B76,CHAR(34),",")</f>
+        <v>pt: "Portuguese",</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="1"/>
         <v>Portuguese (Portugal)(pt-pt)</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G77" t="str">
+        <f>CONCATENATE(E77,": ",CHAR(34),B77,CHAR(34),",")</f>
+        <v>pt-pt: "Portuguese (Portugal)",</v>
+      </c>
+      <c r="H77" t="str">
+        <f>SUBSTITUTE(E77,"-","_")</f>
+        <v>pt_pt</v>
+      </c>
+      <c r="I77" t="str">
+        <f>CONCATENATE(H77,": ",CHAR(34),B77,CHAR(34),",")</f>
+        <v>pt_pt: "Portuguese (Portugal)",</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="1"/>
         <v>Romanian (or Moldavian; or Moldovan)(ro)</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G78" t="str">
+        <f>CONCATENATE(E78,": ",CHAR(34),B78,CHAR(34),",")</f>
+        <v>ro: "Romanian (or Moldavian; or Moldovan)",</v>
+      </c>
+      <c r="H78" t="str">
+        <f>SUBSTITUTE(E78,"-","_")</f>
+        <v>ro</v>
+      </c>
+      <c r="I78" t="str">
+        <f>CONCATENATE(H78,": ",CHAR(34),B78,CHAR(34),",")</f>
+        <v>ro: "Romanian (or Moldavian; or Moldovan)",</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E79" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="1"/>
         <v>Russian(ru)</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G79" t="str">
+        <f>CONCATENATE(E79,": ",CHAR(34),B79,CHAR(34),",")</f>
+        <v>ru: "Russian",</v>
+      </c>
+      <c r="H79" t="str">
+        <f>SUBSTITUTE(E79,"-","_")</f>
+        <v>ru</v>
+      </c>
+      <c r="I79" t="str">
+        <f>CONCATENATE(H79,": ",CHAR(34),B79,CHAR(34),",")</f>
+        <v>ru: "Russian",</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E80" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="1"/>
         <v>Kinyarwanda(rw)</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G80" t="str">
+        <f>CONCATENATE(E80,": ",CHAR(34),B80,CHAR(34),",")</f>
+        <v>rw: "Kinyarwanda",</v>
+      </c>
+      <c r="H80" t="str">
+        <f>SUBSTITUTE(E80,"-","_")</f>
+        <v>rw</v>
+      </c>
+      <c r="I80" t="str">
+        <f>CONCATENATE(H80,": ",CHAR(34),B80,CHAR(34),",")</f>
+        <v>rw: "Kinyarwanda",</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="1"/>
         <v>Slovak(sk)</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G81" t="str">
+        <f>CONCATENATE(E81,": ",CHAR(34),B81,CHAR(34),",")</f>
+        <v>sk: "Slovak",</v>
+      </c>
+      <c r="H81" t="str">
+        <f>SUBSTITUTE(E81,"-","_")</f>
+        <v>sk</v>
+      </c>
+      <c r="I81" t="str">
+        <f>CONCATENATE(H81,": ",CHAR(34),B81,CHAR(34),",")</f>
+        <v>sk: "Slovak",</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="E82" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="1"/>
         <v>Slovenian(sl)</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G82" t="str">
+        <f>CONCATENATE(E82,": ",CHAR(34),B82,CHAR(34),",")</f>
+        <v>sl: "Slovenian",</v>
+      </c>
+      <c r="H82" t="str">
+        <f>SUBSTITUTE(E82,"-","_")</f>
+        <v>sl</v>
+      </c>
+      <c r="I82" t="str">
+        <f>CONCATENATE(H82,": ",CHAR(34),B82,CHAR(34),",")</f>
+        <v>sl: "Slovenian",</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="E83" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="1"/>
         <v>Serbian(sr)</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G83" t="str">
+        <f>CONCATENATE(E83,": ",CHAR(34),B83,CHAR(34),",")</f>
+        <v>sr: "Serbian",</v>
+      </c>
+      <c r="H83" t="str">
+        <f>SUBSTITUTE(E83,"-","_")</f>
+        <v>sr</v>
+      </c>
+      <c r="I83" t="str">
+        <f>CONCATENATE(H83,": ",CHAR(34),B83,CHAR(34),",")</f>
+        <v>sr: "Serbian",</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="C84" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E84" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="1"/>
         <v>Serbian (Latin script)(sr-latn)</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G84" t="str">
+        <f>CONCATENATE(E84,": ",CHAR(34),B84,CHAR(34),",")</f>
+        <v>sr-latn: "Serbian (Latin script)",</v>
+      </c>
+      <c r="H84" t="str">
+        <f>SUBSTITUTE(E84,"-","_")</f>
+        <v>sr_latn</v>
+      </c>
+      <c r="I84" t="str">
+        <f>CONCATENATE(H84,": ",CHAR(34),B84,CHAR(34),",")</f>
+        <v>sr_latn: "Serbian (Latin script)",</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E85" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="1"/>
         <v>Swedish(sv)</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G85" t="str">
+        <f>CONCATENATE(E85,": ",CHAR(34),B85,CHAR(34),",")</f>
+        <v>sv: "Swedish",</v>
+      </c>
+      <c r="H85" t="str">
+        <f>SUBSTITUTE(E85,"-","_")</f>
+        <v>sv</v>
+      </c>
+      <c r="I85" t="str">
+        <f>CONCATENATE(H85,": ",CHAR(34),B85,CHAR(34),",")</f>
+        <v>sv: "Swedish",</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E86" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="1"/>
         <v>Swedish (Finland)(sv-fi)</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G86" t="str">
+        <f>CONCATENATE(E86,": ",CHAR(34),B86,CHAR(34),",")</f>
+        <v>sv-fi: "Swedish (Finland)",</v>
+      </c>
+      <c r="H86" t="str">
+        <f>SUBSTITUTE(E86,"-","_")</f>
+        <v>sv_fi</v>
+      </c>
+      <c r="I86" t="str">
+        <f>CONCATENATE(H86,": ",CHAR(34),B86,CHAR(34),",")</f>
+        <v>sv_fi: "Swedish (Finland)",</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="C87" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E87" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="1"/>
         <v>Turkmen(tk)</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G87" t="str">
+        <f>CONCATENATE(E87,": ",CHAR(34),B87,CHAR(34),",")</f>
+        <v>tk: "Turkmen",</v>
+      </c>
+      <c r="H87" t="str">
+        <f>SUBSTITUTE(E87,"-","_")</f>
+        <v>tk</v>
+      </c>
+      <c r="I87" t="str">
+        <f>CONCATENATE(H87,": ",CHAR(34),B87,CHAR(34),",")</f>
+        <v>tk: "Turkmen",</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="C88" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E88" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="1"/>
         <v>Klingon (or tlhIngan Hol)(tlh)</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G88" t="str">
+        <f>CONCATENATE(E88,": ",CHAR(34),B88,CHAR(34),",")</f>
+        <v>tlh: "Klingon (or tlhIngan Hol)",</v>
+      </c>
+      <c r="H88" t="str">
+        <f>SUBSTITUTE(E88,"-","_")</f>
+        <v>tlh</v>
+      </c>
+      <c r="I88" t="str">
+        <f>CONCATENATE(H88,": ",CHAR(34),B88,CHAR(34),",")</f>
+        <v>tlh: "Klingon (or tlhIngan Hol)",</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="C89" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E89" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="1"/>
         <v>Klingon (or tlhIngan Hol; Latin script)(tlh-latn)</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G89" t="str">
+        <f>CONCATENATE(E89,": ",CHAR(34),B89,CHAR(34),",")</f>
+        <v>tlh-latn: "Klingon (or tlhIngan Hol; Latin script)",</v>
+      </c>
+      <c r="H89" t="str">
+        <f>SUBSTITUTE(E89,"-","_")</f>
+        <v>tlh_latn</v>
+      </c>
+      <c r="I89" t="str">
+        <f>CONCATENATE(H89,": ",CHAR(34),B89,CHAR(34),",")</f>
+        <v>tlh_latn: "Klingon (or tlhIngan Hol; Latin script)",</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="C90" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E90" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="1"/>
         <v>Turkish(tr)</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G90" t="str">
+        <f>CONCATENATE(E90,": ",CHAR(34),B90,CHAR(34),",")</f>
+        <v>tr: "Turkish",</v>
+      </c>
+      <c r="H90" t="str">
+        <f>SUBSTITUTE(E90,"-","_")</f>
+        <v>tr</v>
+      </c>
+      <c r="I90" t="str">
+        <f>CONCATENATE(H90,": ",CHAR(34),B90,CHAR(34),",")</f>
+        <v>tr: "Turkish",</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E91" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="1"/>
         <v>Ukrainian(uk)</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="G91" t="str">
+        <f>CONCATENATE(E91,": ",CHAR(34),B91,CHAR(34),",")</f>
+        <v>uk: "Ukrainian",</v>
+      </c>
+      <c r="H91" t="str">
+        <f>SUBSTITUTE(E91,"-","_")</f>
+        <v>uk</v>
+      </c>
+      <c r="I91" t="str">
+        <f>CONCATENATE(H91,": ",CHAR(34),B91,CHAR(34),",")</f>
+        <v>uk: "Ukrainian",</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E92" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="1"/>
         <v>Vietnamese(vi)</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92" t="str">
+        <f>CONCATENATE(E92,": ",CHAR(34),B92,CHAR(34),",")</f>
+        <v>vi: "Vietnamese",</v>
+      </c>
+      <c r="H92" t="str">
+        <f>SUBSTITUTE(E92,"-","_")</f>
+        <v>vi</v>
+      </c>
+      <c r="I92" t="str">
+        <f>CONCATENATE(H92,": ",CHAR(34),B92,CHAR(34),",")</f>
+        <v>vi: "Vietnamese",</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F93" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93" t="str">
+        <f>CONCATENATE(E93,": ",CHAR(34),B93,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="H93" t="str">
+        <f>SUBSTITUTE(E93,"-","_")</f>
+        <v/>
+      </c>
+      <c r="I93" t="str">
+        <f>CONCATENATE(H93,": ",CHAR(34),B93,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F94" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94" t="str">
+        <f>CONCATENATE(E94,": ",CHAR(34),B94,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="H94" t="str">
+        <f>SUBSTITUTE(E94,"-","_")</f>
+        <v/>
+      </c>
+      <c r="I94" t="str">
+        <f>CONCATENATE(H94,": ",CHAR(34),B94,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F95" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95" t="str">
+        <f>CONCATENATE(E95,": ",CHAR(34),B95,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="H95" t="str">
+        <f>SUBSTITUTE(E95,"-","_")</f>
+        <v/>
+      </c>
+      <c r="I95" t="str">
+        <f>CONCATENATE(H95,": ",CHAR(34),B95,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F96" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G96" t="str">
+        <f>CONCATENATE(E96,": ",CHAR(34),B96,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="H96" t="str">
+        <f>SUBSTITUTE(E96,"-","_")</f>
+        <v/>
+      </c>
+      <c r="I96" t="str">
+        <f>CONCATENATE(H96,": ",CHAR(34),B96,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="97" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F97" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G97" t="str">
+        <f>CONCATENATE(E97,": ",CHAR(34),B97,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I97" t="str">
+        <f>CONCATENATE(H97,": ",CHAR(34),B97,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="98" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F98" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G98" t="str">
+        <f>CONCATENATE(E98,": ",CHAR(34),B98,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I98" t="str">
+        <f>CONCATENATE(H98,": ",CHAR(34),B98,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="99" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F99" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G99" t="str">
+        <f>CONCATENATE(E99,": ",CHAR(34),B99,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I99" t="str">
+        <f>CONCATENATE(H99,": ",CHAR(34),B99,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="100" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F100" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G100" t="str">
+        <f>CONCATENATE(E100,": ",CHAR(34),B100,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I100" t="str">
+        <f>CONCATENATE(H100,": ",CHAR(34),B100,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="101" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F101" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G101" t="str">
+        <f>CONCATENATE(E101,": ",CHAR(34),B101,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I101" t="str">
+        <f>CONCATENATE(H101,": ",CHAR(34),B101,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+    </row>
+    <row r="102" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F102" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G102" t="str">
+        <f>CONCATENATE(E102,": ",CHAR(34),B102,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I102" t="str">
+        <f>CONCATENATE(G102,": ",CHAR(34),D102,CHAR(34),",")</f>
+        <v>: "",: "",</v>
+      </c>
+    </row>
+    <row r="103" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F103" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G103" t="str">
+        <f>CONCATENATE(E103,": ",CHAR(34),B103,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I103" t="str">
+        <f>CONCATENATE(G103,": ",CHAR(34),D103,CHAR(34),",")</f>
+        <v>: "",: "",</v>
+      </c>
+    </row>
+    <row r="104" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F104" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G104" t="str">
+        <f>CONCATENATE(E104,": ",CHAR(34),B104,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I104" t="str">
+        <f>CONCATENATE(G104,": ",CHAR(34),D104,CHAR(34),",")</f>
+        <v>: "",: "",</v>
+      </c>
+    </row>
+    <row r="105" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F105" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G105" t="str">
+        <f>CONCATENATE(E105,": ",CHAR(34),B105,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I105" t="str">
+        <f>CONCATENATE(G105,": ",CHAR(34),D105,CHAR(34),",")</f>
+        <v>: "",: "",</v>
+      </c>
+    </row>
+    <row r="106" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F106" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G106" t="str">
+        <f>CONCATENATE(E106,": ",CHAR(34),B106,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I106" t="str">
+        <f>CONCATENATE(G106,": ",CHAR(34),D106,CHAR(34),",")</f>
+        <v>: "",: "",</v>
+      </c>
+    </row>
+    <row r="107" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F107" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G107" t="str">
+        <f>CONCATENATE(E107,": ",CHAR(34),B107,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I107" t="str">
+        <f>CONCATENATE(G107,": ",CHAR(34),D107,CHAR(34),",")</f>
+        <v>: "",: "",</v>
+      </c>
+    </row>
+    <row r="108" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F108" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
-    </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="G108" t="str">
+        <f>CONCATENATE(E108,": ",CHAR(34),B108,CHAR(34),",")</f>
+        <v>: "",</v>
+      </c>
+      <c r="I108" t="str">
+        <f>CONCATENATE(G108,": ",CHAR(34),D108,CHAR(34),",")</f>
+        <v>: "",: "",</v>
+      </c>
+    </row>
+    <row r="109" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F109" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F110" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F111" t="str">
         <f t="shared" si="1"/>
         <v>()</v>
       </c>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F112" t="str">
         <f t="shared" si="1"/>
         <v>()</v>

</xml_diff>